<commit_message>
remove national and state data and disable sorting function of each column.
</commit_message>
<xml_diff>
--- a/final_initiatives.xlsx
+++ b/final_initiatives.xlsx
@@ -7,16 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="state" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="national" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="530">
-  <si>
-    <t xml:space="preserve">Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="462">
+  <si>
+    <t xml:space="preserve">Initiative Name</t>
   </si>
   <si>
     <t xml:space="preserve">Contact name</t>
@@ -151,6 +149,30 @@
     <t xml:space="preserve">City of Riverside</t>
   </si>
   <si>
+    <t xml:space="preserve">Autism Employment Collaborative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beth Burt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bburt@ieautism.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The autism community has a 96% unemployment rate. The Autism Society Inland Empire Working together with our partners such as Inland Regional Center, Department of Rehabilitation, and the State Council on Developmental Disabilities - the Autism Employment Collaborative was born with a focus for improving these outcomes. This included looking at systems to create innovative service to promote accountability, creativity, and stable and sufficient funding streams to support person-centered, meaningful lives.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Autism Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonprofits - advocates / base builders, Nonprofits - service providers, Govt agency - State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ieautism.org/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Black Equity Initiative of the IE</t>
   </si>
   <si>
@@ -229,9 +251,6 @@
     <t xml:space="preserve">UC Riverside has received a $16-million grand from the National Institutes of Health to help reduce health disparities, particularly among Latinos who make up about half the region’s population. The five-year grant will allow the university’s School of Medicine to launch the Center for Health Disparities Research — an effort that will bring together researchers in the environmental, biomedical and social sciences fields. The new center will use a “community-based approach” to evaluate and improve the health of underserved communities in the Inland Empire.</t>
   </si>
   <si>
-    <t xml:space="preserve">Health Equity</t>
-  </si>
-  <si>
     <t xml:space="preserve">UC Riverside</t>
   </si>
   <si>
@@ -239,6 +258,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://medschool.ucr.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLASE (Colaboración, Liderazgo, Abogacía, Servicio y Educación (CLASE) Community of Practice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Autism Society Inland Empire founded CLASE (Colaboración, Liderazgo, Abogacía, Servicio y Educación (CLASE) Community of Practice. This Latino Community of Practice includes 33 leaders from 19 CBOs that serve Hispanic and Spanish speaking individuals and families with intellectual and developmental disabilities (I/DD).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hispanic / Latino / Latinx communities,People with disabilities, Undocumented individuals and families,</t>
   </si>
   <si>
     <t xml:space="preserve">College Exodus Project</t>
@@ -1370,241 +1398,7 @@
     <t xml:space="preserve">https://www.gosbcta.com/project/diesel-multiple-unit-to-zero-emission-multiple-unit-pilot/</t>
   </si>
   <si>
-    <t xml:space="preserve">California Advancing and Innovating Medi-Cal Initiative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CalAIM@dhcs.ca.gov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CalAIM is a multi-year initiative by DHCS to improve the quality of life and health outcomes of our population by implementing broad delivery system, program and payment reform across the Medi-Cal program. The major components of CalAIM build upon the successful outcomes of various pilots (including but not limited to the Whole Person Care Pilots (WPC), Health Homes Program (HHP), and the Coordinated Care Initiative) from the previous federal waivers and will result in a better quality of life for Medi-Cal members as well as long-term cost savings/avoidance. CalAIM has three primary goals: Identify and manage member risk and need through whole person care approaches and addressing Social Determinants of Health; Move Medi-Cal to a more consistent and seamless system by reducing complexity and increasing flexibility; and Improve quality outcomes, reduce health disparities, and drive delivery system transformation and innovation through value-based initiatives, modernization of systems, and payment reform.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State of California</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statewide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large businesses, Small businesses, Nonprofits - advocates / base builders, Nonprofits - service providers, Govt agency - Federal, Govt agency - State, Govt agency - Local, Philanthropy - national funder, Philanthropy - state funder, Philanthropy - local funder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.dhcs.ca.gov/provgovpart/Pages/CalAIM.aspx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">California Five-Year Infrastructure Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The components of the five year infrastructure plan includes: economic recovery, climate resilience, broadband, and education. The plan reviews the budget allocation for these projects. Their focus is on building resilient infrastructure through investments in state’s capital assets.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Office of Governor Newsom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Department of State Finance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campaign for College Opportunity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info@collegecampaign.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Campaign for College Opportunity’s mission has been to ensure that all eligible and motivated students in California have an opportunity to go to college and succeed. The Campaign remains committed to keeping the State of California from breaking its promise of college opportunity to its next generation of young people in order to ensure a strong state for all of us.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Academic / colleges or universities, Large businesses, Small businesses, Nonprofits - advocates / base builders, Nonprofits - service providers, Govt agency - Federal, Govt agency - State, Govt agency - Local, Philanthropy - national funder, Philanthropy - state funder, Philanthropy - local funder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://collegecampaign.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closing the Digital Divide Initiative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Divide Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">digitaldivide@cde.ca.gov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Closing the Digital Divide Initiative focuses on identifying needed resources and partnerships to support distance learning in California schools and equip all California students with computing devices and connectivity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">California Department of Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Academic / colleges or universities, Large businesses, Nonprofits - advocates / base builders, Nonprofits - service providers, Govt agency - Federal, Govt agency - State, Govt agency - Local, Other health providers, Philanthropy - national funder, Philanthropy - state funder, Philanthropy - local funder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Having Our Say Coalition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info@cpehn.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Having Our Say coalition was founded in 2007 to raise the voices of communities of color in the health reform debate and to advocate for access to quality health care for all. Three years later, the Patient Protection and Affordable Care Act (ACA) was signed into law and 3.4 million previously uninsured California residents received health care insurance, some for the very first time. In 2015, thanks to the hard work of advocates, California expanded Medi-Cal to cover all low-income children, regardless of their immigration status. An estimated 250,000 undocumented children enrolled. We have since expanded Medi-Cal coverage to all undocumented youth in 2019 and have continued to advocate for the right to health for all, including addressing systemic racism and injustices that disproportionally impact communities of color and directly lead to health disparities.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">California Pan Ethnic Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cpehn.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keeping Seniors Healthy and Independent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercedes Perezchica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mperezchica@scanhealthplan.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Independence at Home (IAH), a SCAN community service, provides no-cost programs. support and resource referrals for older adults and caregivers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital divide, Health and Health Equity, Transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCAN Health Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 CA Counties: Los Angeles County, Napa County, Orange County, Riverside County, San Bernardino County, San Diego County, San Francisco County, Santa Clara County, Sonoma County, Stanislaus County, and Ventura County.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nonprofits - service providers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black communities, American Indian / Native / Indigenous communities, Asian American communities, Hispanic / Latino / Latinx communities, Homelessness/Housing insecurity, Native Hawaiian / Pacific Islander communities, Elders / seniors, LGBTQ+ communities, Low-income residents, People with disabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://independenceathome.org/our-services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Supports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Let's Get Health California</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Let’s Get Healthy California provides an ongoing statewide collaborative and systematic approach for assessing and monitoring the health status of California, identifying and prioritizing opportunities for health improvement, and promoting collective action towards comprehensive solutions that address the root causes of California’s toughest health challenges.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network of Promotoras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria Lemus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maria@visionycompromiso.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In 2001 we established the first and only Network of Promotoras and Community Health Workers in California. The Network now includes more than 4,000 promotores in 13 regions of California and one region in Mexico. In 2015 we also expanded to a National Network to include additional community networks in five states: Washington, Oregon, Colorado, Nevada, and Arizona. The Network provides leadership, training and advocacy for promotores and community health workers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civic Engagement, Economic Development, Health and Health Equity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vision y Compromiso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Academic / colleges or universities, Nonprofits - advocates / base builders, Nonprofits - service providers, Govt agency - Federal, Govt agency - State, Govt agency - Local, Community clinics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic / Latino / Latinx communities, Low-income residents, Undocumented individuals and families, Women</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://visionycompromiso.org/what-we-do/the-network/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID testing, Mutual aid, Food assistance, Voter engagement, Census outreach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Homekey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HomeKey@hcd.ca.gov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Building on the success of Project Roomkey Opens in New Window, Homekey is the next phase in the state’s response to protecting Californians experiencing homelessness who are at high risk for serious illness and are impacted by COVID-19. Administered by the California Department of Housing and Community Development (HCD), $600 million in grant funding will be made available to local public entities, including cities, counties, or other local public entities, including housing authorities or federally recognized tribal governments within California to purchase and rehabilitate housing, including hotels, motels, vacant apartment buildings, and other buildings and convert them into interim or permanent, long-term housing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">California Department of Housing and Community Development (HCD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.hcd.ca.gov/grants-funding/active-funding/homekey.shtml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regions Rise Together</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egon Terplan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egon.terplan@sgc.ca.gov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regions Rise Together offers a high road vision for inclusive and resilient economic development, and sustainable land use and transportation planning, across California and its regions, recognizing both their diversity and interconnectedness. Launched in 2019 with the Governor’s Office of Business and Economic Development, Regions Rise Together is changing the mental map of the state by drawing attention to opportunities and assets in all regions, especially inland California. Regions Rise Together is actively partnering on regions-up economic diversification strategies across California’s regions. These economic development strategies are a part of the state’s Just Transition strategy to a carbon neutral economy, which encourages each region to build on existing assets and grow quality jobs in new and emerging high road industries.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Governor's Office of Planning and Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.arcgis.com/apps/Cascade/index.html?appid=d056b93e3116413cbd1ad25cc4245221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020 National Recreation Movement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rosario Galeas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rperez@latinohealthaccess.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Recreation Movement community is commited to growing individual and community wellbeing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food Systems, Health and Health Equity, Media, Nonprofit Equity, Public Safety, Youth Development &amp; Empowerment, Workforce Development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIRSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Academic / colleges or universities, Large businesses, Govt agency - Federal, Govt agency - State, Other health providers, Media (ethnic or community-specific media)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Youth/Students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://recmovement.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID testing, Other health services, Food assistance, Voter registration, Voter engagement, Census outreach, Diabetes Prevention, and Mental Health Services.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complete College America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandon Protas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bprotas@completecollege.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complete College America is restoring the promise of higher education by advocating for forward-thinking policies, identifying effective strategies, and advancing proven tactics that guarantee more students earn college diplomas or credentials that prepare them for success.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Academic / colleges or universities, Nonprofits - advocates / base builders, Nonprofits - service providers, Govt agency - Federal, Govt agency - State, Govt agency - Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://completecollege.org/</t>
+    <t xml:space="preserve">Individuals who have autism are seven times more likely to have interactions with police. The news is full of tragic stories of individuals with autism who have been shot or arrested. The Autism Society Inland Empire applied for and received a grant from the California Police Officer Standards &amp; Training in 2020. A 4-hour Autism &amp; Developmental Disabilities Curriculum was developed and this training is now being piloted to 240 officers in San Bernardino and Riverside Counties. If adopted, it will be used throughout California.</t>
   </si>
 </sst>
 </file>
@@ -1687,50 +1481,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A12:K76" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A12:K76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A12:K79" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A12:K79"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Contact name"/>
-    <tableColumn id="3" name="Contact email"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Area of focus"/>
-    <tableColumn id="6" name="Org Lead"/>
-    <tableColumn id="7" name="Geo scope"/>
-    <tableColumn id="8" name="Partners"/>
-    <tableColumn id="9" name="Priority population"/>
-    <tableColumn id="10" name="URL"/>
-    <tableColumn id="11" name="Additional Info"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K11" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K11"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Contact name"/>
-    <tableColumn id="3" name="Contact email"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Area of focus"/>
-    <tableColumn id="6" name="Org Lead"/>
-    <tableColumn id="7" name="Geo scope"/>
-    <tableColumn id="8" name="Partners"/>
-    <tableColumn id="9" name="Priority population"/>
-    <tableColumn id="10" name="URL"/>
-    <tableColumn id="11" name="Additional Info"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:K3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K3"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="Name"/>
+    <tableColumn id="1" name="Initiative Name"/>
     <tableColumn id="2" name="Contact name"/>
     <tableColumn id="3" name="Contact email"/>
     <tableColumn id="4" name="Description"/>
@@ -2207,20 +1961,18 @@
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
         <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" t="s">
         <v>51</v>
       </c>
+      <c r="I17"/>
       <c r="J17" t="s">
         <v>52</v>
       </c>
@@ -2240,47 +1992,47 @@
         <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
         <v>57</v>
       </c>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>59</v>
+      </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" t="s">
         <v>65</v>
       </c>
-      <c r="I19" t="s">
-        <v>30</v>
-      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
       <c r="J19" t="s">
         <v>66</v>
       </c>
@@ -2306,7 +2058,7 @@
         <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H20" t="s">
         <v>73</v>
@@ -2333,667 +2085,667 @@
         <v>78</v>
       </c>
       <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="s">
         <v>79</v>
-      </c>
-      <c r="F21" t="s">
-        <v>80</v>
       </c>
       <c r="G21" t="s">
         <v>17</v>
       </c>
       <c r="H21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" t="s">
         <v>81</v>
-      </c>
-      <c r="I21" t="s">
-        <v>82</v>
-      </c>
-      <c r="J21" t="s">
-        <v>83</v>
       </c>
       <c r="K21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="G22" t="s">
         <v>17</v>
       </c>
       <c r="H22"/>
-      <c r="I22"/>
+      <c r="I22" t="s">
+        <v>84</v>
+      </c>
       <c r="J22" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="K22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" t="s">
         <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" t="s">
-        <v>95</v>
       </c>
       <c r="G23" t="s">
         <v>17</v>
       </c>
       <c r="H23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J23" t="s">
-        <v>98</v>
-      </c>
-      <c r="K23" t="s">
-        <v>99</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24"/>
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G24" t="s">
         <v>17</v>
       </c>
-      <c r="H24" t="s">
-        <v>104</v>
-      </c>
-      <c r="I24" t="s">
-        <v>105</v>
-      </c>
+      <c r="H24"/>
+      <c r="I24"/>
       <c r="J24" t="s">
-        <v>106</v>
-      </c>
-      <c r="K24" t="s">
-        <v>107</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="K24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" t="s">
+        <v>107</v>
+      </c>
+      <c r="J25" t="s">
         <v>108</v>
       </c>
-      <c r="B25" t="s">
+      <c r="K25" t="s">
         <v>109</v>
       </c>
-      <c r="C25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" t="s">
-        <v>113</v>
-      </c>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25" t="s">
-        <v>114</v>
-      </c>
-      <c r="K25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" t="s">
-        <v>118</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D26"/>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G26" t="s">
         <v>17</v>
       </c>
       <c r="H26" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I26" t="s">
-        <v>30</v>
+        <v>115</v>
       </c>
       <c r="J26" t="s">
-        <v>121</v>
-      </c>
-      <c r="K26"/>
+        <v>116</v>
+      </c>
+      <c r="K26" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
         <v>122</v>
       </c>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27"/>
+      <c r="G27" t="s">
+        <v>123</v>
+      </c>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27"/>
+      <c r="J27" t="s">
+        <v>124</v>
+      </c>
       <c r="K27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28"/>
+        <v>125</v>
+      </c>
+      <c r="B28" t="s">
+        <v>126</v>
+      </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G28" t="s">
         <v>17</v>
       </c>
       <c r="H28" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I28" t="s">
         <v>30</v>
       </c>
       <c r="J28" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="K28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" t="s">
         <v>132</v>
       </c>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
       <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" t="s">
-        <v>133</v>
-      </c>
-      <c r="G29" t="s">
-        <v>17</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
-      <c r="J29" t="s">
-        <v>134</v>
-      </c>
+      <c r="J29"/>
       <c r="K29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30"/>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" t="s">
         <v>135</v>
       </c>
-      <c r="B30" t="s">
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" t="s">
         <v>136</v>
       </c>
-      <c r="C30" t="s">
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="s">
         <v>137</v>
       </c>
-      <c r="D30" t="s">
+      <c r="I30" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" t="s">
         <v>138</v>
-      </c>
-      <c r="E30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G30" t="s">
-        <v>113</v>
-      </c>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30" t="s">
-        <v>139</v>
       </c>
       <c r="K30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" t="s">
         <v>140</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>141</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>142</v>
-      </c>
-      <c r="D31" t="s">
-        <v>143</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G31" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" t="s">
         <v>147</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>148</v>
-      </c>
-      <c r="C32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D32" t="s">
-        <v>150</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G32" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" t="s">
         <v>152</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>153</v>
-      </c>
-      <c r="C33" t="s">
-        <v>154</v>
-      </c>
-      <c r="D33" t="s">
-        <v>155</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
       </c>
       <c r="F33" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" t="s">
+        <v>155</v>
+      </c>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33" t="s">
         <v>156</v>
       </c>
-      <c r="G33" t="s">
-        <v>157</v>
-      </c>
-      <c r="H33" t="s">
-        <v>158</v>
-      </c>
-      <c r="I33" t="s">
-        <v>159</v>
-      </c>
-      <c r="J33" t="s">
-        <v>160</v>
-      </c>
-      <c r="K33" t="s">
-        <v>161</v>
-      </c>
+      <c r="K33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C34" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="G34" t="s">
-        <v>167</v>
-      </c>
-      <c r="H34" t="s">
-        <v>168</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="H34"/>
       <c r="I34"/>
       <c r="J34" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>166</v>
+      </c>
+      <c r="G35" t="s">
+        <v>167</v>
+      </c>
+      <c r="H35" t="s">
+        <v>168</v>
+      </c>
+      <c r="I35" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35" t="s">
         <v>170</v>
       </c>
-      <c r="B35" t="s">
+      <c r="K35" t="s">
         <v>171</v>
       </c>
-      <c r="C35" t="s">
-        <v>172</v>
-      </c>
-      <c r="D35" t="s">
-        <v>173</v>
-      </c>
-      <c r="E35" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35" t="s">
-        <v>170</v>
-      </c>
-      <c r="G35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" t="s">
-        <v>174</v>
-      </c>
-      <c r="I35" t="s">
-        <v>30</v>
-      </c>
-      <c r="J35" t="s">
-        <v>175</v>
-      </c>
-      <c r="K35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B36" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G36" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H36" t="s">
-        <v>182</v>
-      </c>
-      <c r="I36" t="s">
-        <v>183</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="I36"/>
       <c r="J36" t="s">
-        <v>184</v>
-      </c>
-      <c r="K36" t="s">
-        <v>185</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="K36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="F37" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G37" t="s">
         <v>17</v>
       </c>
-      <c r="H37"/>
-      <c r="I37"/>
+      <c r="H37" t="s">
+        <v>184</v>
+      </c>
+      <c r="I37" t="s">
+        <v>30</v>
+      </c>
       <c r="J37" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="K37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" t="s">
+        <v>187</v>
+      </c>
+      <c r="C38" t="s">
         <v>188</v>
       </c>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
+      <c r="D38" t="s">
+        <v>189</v>
+      </c>
       <c r="E38" t="s">
         <v>15</v>
       </c>
       <c r="F38" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G38" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
+        <v>191</v>
+      </c>
+      <c r="H38" t="s">
+        <v>192</v>
+      </c>
+      <c r="I38" t="s">
+        <v>193</v>
+      </c>
+      <c r="J38" t="s">
+        <v>194</v>
+      </c>
+      <c r="K38" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39"/>
+        <v>196</v>
+      </c>
+      <c r="B39" t="s">
+        <v>181</v>
+      </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E39" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="G39" t="s">
-        <v>44</v>
-      </c>
-      <c r="H39" t="s">
-        <v>194</v>
-      </c>
-      <c r="I39" t="s">
-        <v>30</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H39"/>
+      <c r="I39"/>
       <c r="J39" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="K39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>196</v>
-      </c>
-      <c r="B40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C40" t="s">
         <v>198</v>
       </c>
-      <c r="D40" t="s">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
         <v>199</v>
       </c>
-      <c r="E40" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" t="s">
-        <v>200</v>
-      </c>
       <c r="G40" t="s">
-        <v>201</v>
-      </c>
-      <c r="H40" t="s">
-        <v>202</v>
-      </c>
-      <c r="I40" t="s">
-        <v>203</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H40"/>
+      <c r="I40"/>
       <c r="J40"/>
-      <c r="K40" t="s">
-        <v>204</v>
-      </c>
+      <c r="K40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>205</v>
-      </c>
-      <c r="B41" t="s">
-        <v>206</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="B41"/>
       <c r="C41" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D41" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
       <c r="F41" t="s">
-        <v>205</v>
+        <v>44</v>
       </c>
       <c r="G41" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="H41" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I41" t="s">
         <v>30</v>
       </c>
       <c r="J41" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="K41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" t="s">
+        <v>208</v>
+      </c>
+      <c r="D42" t="s">
+        <v>209</v>
+      </c>
+      <c r="E42" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" t="s">
+        <v>210</v>
+      </c>
+      <c r="G42" t="s">
         <v>211</v>
       </c>
-      <c r="B42" t="s">
+      <c r="H42" t="s">
         <v>212</v>
       </c>
-      <c r="C42" t="s">
+      <c r="I42" t="s">
         <v>213</v>
       </c>
-      <c r="D42" t="s">
+      <c r="J42"/>
+      <c r="K42" t="s">
         <v>214</v>
       </c>
-      <c r="E42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" t="s">
-        <v>28</v>
-      </c>
-      <c r="H42" t="s">
-        <v>29</v>
-      </c>
-      <c r="I42" t="s">
-        <v>30</v>
-      </c>
-      <c r="J42" t="s">
-        <v>215</v>
-      </c>
-      <c r="K42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>215</v>
+      </c>
+      <c r="B43" t="s">
         <v>216</v>
       </c>
-      <c r="B43"/>
       <c r="C43" t="s">
         <v>217</v>
       </c>
@@ -3004,87 +2756,83 @@
         <v>15</v>
       </c>
       <c r="F43" t="s">
+        <v>215</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="s">
         <v>219</v>
       </c>
-      <c r="G43" t="s">
+      <c r="I43" t="s">
+        <v>30</v>
+      </c>
+      <c r="J43" t="s">
         <v>220</v>
-      </c>
-      <c r="H43" t="s">
-        <v>221</v>
-      </c>
-      <c r="I43" t="s">
-        <v>222</v>
-      </c>
-      <c r="J43" t="s">
-        <v>223</v>
       </c>
       <c r="K43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" t="s">
+        <v>222</v>
+      </c>
+      <c r="C44" t="s">
+        <v>223</v>
+      </c>
+      <c r="D44" t="s">
         <v>224</v>
       </c>
-      <c r="B44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J44" t="s">
         <v>225</v>
       </c>
-      <c r="D44" t="s">
-        <v>226</v>
-      </c>
-      <c r="E44" t="s">
-        <v>79</v>
-      </c>
-      <c r="F44" t="s">
-        <v>80</v>
-      </c>
-      <c r="G44" t="s">
-        <v>227</v>
-      </c>
-      <c r="H44" t="s">
-        <v>228</v>
-      </c>
-      <c r="I44" t="s">
-        <v>51</v>
-      </c>
-      <c r="J44" t="s">
-        <v>229</v>
-      </c>
-      <c r="K44" t="s">
-        <v>230</v>
-      </c>
+      <c r="K44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>226</v>
+      </c>
+      <c r="B45"/>
+      <c r="C45" t="s">
+        <v>227</v>
+      </c>
+      <c r="D45" t="s">
+        <v>228</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>229</v>
+      </c>
+      <c r="G45" t="s">
+        <v>230</v>
+      </c>
+      <c r="H45" t="s">
         <v>231</v>
       </c>
-      <c r="B45" t="s">
+      <c r="I45" t="s">
         <v>232</v>
       </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="J45" t="s">
         <v>233</v>
-      </c>
-      <c r="E45" t="s">
-        <v>43</v>
-      </c>
-      <c r="F45" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" t="s">
-        <v>17</v>
-      </c>
-      <c r="H45" t="s">
-        <v>50</v>
-      </c>
-      <c r="I45" t="s">
-        <v>51</v>
-      </c>
-      <c r="J45" t="s">
-        <v>52</v>
       </c>
       <c r="K45"/>
     </row>
@@ -3093,33 +2841,35 @@
         <v>234</v>
       </c>
       <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
         <v>235</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>236</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46" t="s">
         <v>237</v>
       </c>
-      <c r="E46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="H46" t="s">
         <v>238</v>
       </c>
-      <c r="G46" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
+        <v>59</v>
+      </c>
+      <c r="J46" t="s">
         <v>239</v>
       </c>
-      <c r="I46" t="s">
-        <v>30</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>240</v>
       </c>
-      <c r="K46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
@@ -3129,975 +2879,1068 @@
         <v>242</v>
       </c>
       <c r="C47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" t="s">
         <v>243</v>
       </c>
-      <c r="D47" t="s">
-        <v>244</v>
-      </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>245</v>
+        <v>57</v>
       </c>
       <c r="G47" t="s">
         <v>17</v>
       </c>
       <c r="H47" t="s">
-        <v>246</v>
+        <v>58</v>
       </c>
       <c r="I47" t="s">
-        <v>247</v>
+        <v>59</v>
       </c>
       <c r="J47" t="s">
-        <v>248</v>
+        <v>60</v>
       </c>
       <c r="K47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>244</v>
+      </c>
+      <c r="B48" t="s">
+        <v>245</v>
+      </c>
+      <c r="C48" t="s">
+        <v>246</v>
+      </c>
+      <c r="D48" t="s">
+        <v>247</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>248</v>
+      </c>
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="s">
         <v>249</v>
       </c>
-      <c r="B48" t="s">
+      <c r="I48" t="s">
+        <v>30</v>
+      </c>
+      <c r="J48" t="s">
         <v>250</v>
       </c>
-      <c r="C48" t="s">
-        <v>251</v>
-      </c>
-      <c r="D48" t="s">
-        <v>252</v>
-      </c>
-      <c r="E48" t="s">
-        <v>193</v>
-      </c>
-      <c r="F48"/>
-      <c r="G48" t="s">
-        <v>253</v>
-      </c>
-      <c r="H48" t="s">
-        <v>254</v>
-      </c>
-      <c r="I48" t="s">
-        <v>255</v>
-      </c>
-      <c r="J48" t="s">
-        <v>256</v>
-      </c>
-      <c r="K48" t="s">
-        <v>257</v>
-      </c>
+      <c r="K48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>251</v>
+      </c>
+      <c r="B49" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" t="s">
+        <v>253</v>
+      </c>
+      <c r="D49" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" t="s">
+        <v>255</v>
+      </c>
+      <c r="G49" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I49" t="s">
+        <v>257</v>
+      </c>
+      <c r="J49" t="s">
         <v>258</v>
       </c>
-      <c r="B49" t="s">
-        <v>259</v>
-      </c>
-      <c r="C49" t="s">
-        <v>260</v>
-      </c>
-      <c r="D49" t="s">
-        <v>261</v>
-      </c>
-      <c r="E49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" t="s">
-        <v>262</v>
-      </c>
-      <c r="G49" t="s">
-        <v>263</v>
-      </c>
-      <c r="H49" t="s">
-        <v>264</v>
-      </c>
-      <c r="I49" t="s">
-        <v>265</v>
-      </c>
-      <c r="J49" t="s">
-        <v>266</v>
-      </c>
-      <c r="K49" t="s">
-        <v>267</v>
-      </c>
+      <c r="K49"/>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C50" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D50" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="E50" t="s">
-        <v>15</v>
-      </c>
-      <c r="F50" t="s">
-        <v>272</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="F50"/>
       <c r="G50" t="s">
-        <v>17</v>
-      </c>
-      <c r="H50"/>
-      <c r="I50"/>
+        <v>263</v>
+      </c>
+      <c r="H50" t="s">
+        <v>264</v>
+      </c>
+      <c r="I50" t="s">
+        <v>265</v>
+      </c>
       <c r="J50" t="s">
-        <v>273</v>
-      </c>
-      <c r="K50"/>
+        <v>266</v>
+      </c>
+      <c r="K50" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>268</v>
+      </c>
+      <c r="B51" t="s">
+        <v>269</v>
+      </c>
+      <c r="C51" t="s">
+        <v>270</v>
+      </c>
+      <c r="D51" t="s">
+        <v>271</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" t="s">
+        <v>272</v>
+      </c>
+      <c r="G51" t="s">
+        <v>273</v>
+      </c>
+      <c r="H51" t="s">
         <v>274</v>
       </c>
-      <c r="B51"/>
-      <c r="C51" t="s">
+      <c r="I51" t="s">
         <v>275</v>
       </c>
-      <c r="D51" t="s">
+      <c r="J51" t="s">
         <v>276</v>
       </c>
-      <c r="E51" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51"/>
-      <c r="G51" t="s">
+      <c r="K51" t="s">
         <v>277</v>
       </c>
-      <c r="H51" t="s">
-        <v>239</v>
-      </c>
-      <c r="I51" t="s">
-        <v>30</v>
-      </c>
-      <c r="J51" t="s">
-        <v>278</v>
-      </c>
-      <c r="K51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>278</v>
+      </c>
+      <c r="B52" t="s">
         <v>279</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>280</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>281</v>
-      </c>
-      <c r="D52" t="s">
-        <v>282</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G52" t="s">
         <v>17</v>
       </c>
-      <c r="H52" t="s">
-        <v>284</v>
-      </c>
-      <c r="I52" t="s">
-        <v>285</v>
-      </c>
+      <c r="H52"/>
+      <c r="I52"/>
       <c r="J52" t="s">
-        <v>286</v>
-      </c>
-      <c r="K52" t="s">
-        <v>185</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="K52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>287</v>
-      </c>
-      <c r="B53" t="s">
-        <v>288</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="B53"/>
       <c r="C53" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D53" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
       </c>
-      <c r="F53" t="s">
-        <v>291</v>
-      </c>
+      <c r="F53"/>
       <c r="G53" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H53" t="s">
-        <v>293</v>
-      </c>
-      <c r="I53"/>
+        <v>249</v>
+      </c>
+      <c r="I53" t="s">
+        <v>30</v>
+      </c>
       <c r="J53" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="K53"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B54" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C54" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D54" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G54" t="s">
-        <v>113</v>
-      </c>
-      <c r="H54"/>
-      <c r="I54"/>
+        <v>17</v>
+      </c>
+      <c r="H54" t="s">
+        <v>294</v>
+      </c>
+      <c r="I54" t="s">
+        <v>295</v>
+      </c>
       <c r="J54" t="s">
-        <v>300</v>
-      </c>
-      <c r="K54"/>
+        <v>296</v>
+      </c>
+      <c r="K54" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B55" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C55" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D55" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>32</v>
+        <v>301</v>
       </c>
       <c r="G55" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H55" t="s">
-        <v>306</v>
-      </c>
-      <c r="I55" t="s">
-        <v>307</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="I55"/>
       <c r="J55" t="s">
-        <v>39</v>
-      </c>
-      <c r="K55" t="s">
-        <v>308</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K55"/>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>305</v>
+      </c>
+      <c r="B56" t="s">
+        <v>306</v>
+      </c>
+      <c r="C56" t="s">
+        <v>307</v>
+      </c>
+      <c r="D56" t="s">
+        <v>308</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
         <v>309</v>
       </c>
-      <c r="B56" t="s">
+      <c r="G56" t="s">
+        <v>123</v>
+      </c>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56" t="s">
         <v>310</v>
       </c>
-      <c r="C56" t="s">
-        <v>311</v>
-      </c>
-      <c r="D56" t="s">
-        <v>312</v>
-      </c>
-      <c r="E56" t="s">
-        <v>193</v>
-      </c>
-      <c r="F56" t="s">
-        <v>313</v>
-      </c>
-      <c r="G56" t="s">
-        <v>314</v>
-      </c>
-      <c r="H56" t="s">
-        <v>315</v>
-      </c>
-      <c r="I56" t="s">
-        <v>316</v>
-      </c>
-      <c r="J56" t="s">
-        <v>317</v>
-      </c>
-      <c r="K56" t="s">
-        <v>318</v>
-      </c>
+      <c r="K56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B57" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C57" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D57" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
       </c>
       <c r="F57" t="s">
-        <v>323</v>
+        <v>32</v>
       </c>
       <c r="G57" t="s">
-        <v>201</v>
+        <v>315</v>
       </c>
       <c r="H57" t="s">
-        <v>81</v>
+        <v>316</v>
       </c>
       <c r="I57" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="J57" t="s">
-        <v>325</v>
-      </c>
-      <c r="K57"/>
+        <v>39</v>
+      </c>
+      <c r="K57" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>319</v>
+      </c>
+      <c r="B58" t="s">
+        <v>320</v>
+      </c>
+      <c r="C58" t="s">
+        <v>321</v>
+      </c>
+      <c r="D58" t="s">
+        <v>322</v>
+      </c>
+      <c r="E58" t="s">
+        <v>203</v>
+      </c>
+      <c r="F58" t="s">
+        <v>323</v>
+      </c>
+      <c r="G58" t="s">
+        <v>324</v>
+      </c>
+      <c r="H58" t="s">
+        <v>325</v>
+      </c>
+      <c r="I58" t="s">
         <v>326</v>
       </c>
-      <c r="B58" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58" t="s">
-        <v>92</v>
-      </c>
-      <c r="D58"/>
-      <c r="E58" t="s">
-        <v>94</v>
-      </c>
-      <c r="F58" t="s">
-        <v>95</v>
-      </c>
-      <c r="G58" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" t="s">
-        <v>96</v>
-      </c>
-      <c r="I58" t="s">
-        <v>30</v>
-      </c>
       <c r="J58" t="s">
-        <v>98</v>
-      </c>
-      <c r="K58"/>
+        <v>327</v>
+      </c>
+      <c r="K58" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>330</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>331</v>
       </c>
       <c r="D59" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="E59" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>103</v>
+        <v>333</v>
       </c>
       <c r="G59" t="s">
-        <v>277</v>
-      </c>
-      <c r="H59"/>
-      <c r="I59"/>
+        <v>211</v>
+      </c>
+      <c r="H59" t="s">
+        <v>91</v>
+      </c>
+      <c r="I59" t="s">
+        <v>334</v>
+      </c>
       <c r="J59" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="K59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B60" t="s">
-        <v>331</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>332</v>
+        <v>102</v>
       </c>
       <c r="D60"/>
       <c r="E60" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="F60" t="s">
-        <v>333</v>
+        <v>105</v>
       </c>
       <c r="G60" t="s">
-        <v>292</v>
+        <v>17</v>
       </c>
       <c r="H60" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
       <c r="I60" t="s">
         <v>30</v>
       </c>
       <c r="J60" t="s">
-        <v>334</v>
+        <v>108</v>
       </c>
       <c r="K60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B61" t="s">
-        <v>336</v>
+        <v>111</v>
       </c>
       <c r="C61" t="s">
-        <v>337</v>
+        <v>112</v>
       </c>
       <c r="D61" t="s">
         <v>338</v>
       </c>
       <c r="E61" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>339</v>
+        <v>113</v>
       </c>
       <c r="G61" t="s">
-        <v>17</v>
-      </c>
-      <c r="H61" t="s">
-        <v>340</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="H61"/>
       <c r="I61"/>
       <c r="J61" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>340</v>
+      </c>
+      <c r="B62" t="s">
+        <v>341</v>
+      </c>
+      <c r="C62" t="s">
         <v>342</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62"/>
+      <c r="E62" t="s">
+        <v>49</v>
+      </c>
+      <c r="F62" t="s">
         <v>343</v>
       </c>
-      <c r="C62" t="s">
+      <c r="G62" t="s">
+        <v>302</v>
+      </c>
+      <c r="H62" t="s">
+        <v>219</v>
+      </c>
+      <c r="I62" t="s">
+        <v>30</v>
+      </c>
+      <c r="J62" t="s">
         <v>344</v>
       </c>
-      <c r="D62" t="s">
-        <v>345</v>
-      </c>
-      <c r="E62" t="s">
-        <v>15</v>
-      </c>
-      <c r="F62" t="s">
-        <v>72</v>
-      </c>
-      <c r="G62" t="s">
-        <v>346</v>
-      </c>
-      <c r="H62" t="s">
-        <v>347</v>
-      </c>
-      <c r="I62" t="s">
-        <v>348</v>
-      </c>
-      <c r="J62" t="s">
-        <v>349</v>
-      </c>
-      <c r="K62" t="s">
-        <v>350</v>
-      </c>
+      <c r="K62"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B63" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C63" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D63" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
       </c>
       <c r="F63" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="G63" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H63" t="s">
-        <v>356</v>
-      </c>
-      <c r="I63" t="s">
-        <v>357</v>
-      </c>
-      <c r="J63"/>
-      <c r="K63" t="s">
-        <v>358</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="I63"/>
+      <c r="J63" t="s">
+        <v>351</v>
+      </c>
+      <c r="K63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>352</v>
+      </c>
+      <c r="B64" t="s">
+        <v>353</v>
+      </c>
+      <c r="C64" t="s">
+        <v>354</v>
+      </c>
+      <c r="D64" t="s">
+        <v>355</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>79</v>
+      </c>
+      <c r="G64" t="s">
+        <v>356</v>
+      </c>
+      <c r="H64" t="s">
+        <v>357</v>
+      </c>
+      <c r="I64" t="s">
+        <v>358</v>
+      </c>
+      <c r="J64" t="s">
         <v>359</v>
       </c>
-      <c r="B64" t="s">
+      <c r="K64" t="s">
         <v>360</v>
-      </c>
-      <c r="C64" t="s">
-        <v>361</v>
-      </c>
-      <c r="D64" t="s">
-        <v>362</v>
-      </c>
-      <c r="E64" t="s">
-        <v>79</v>
-      </c>
-      <c r="F64" t="s">
-        <v>363</v>
-      </c>
-      <c r="G64" t="s">
-        <v>292</v>
-      </c>
-      <c r="H64" t="s">
-        <v>209</v>
-      </c>
-      <c r="I64" t="s">
-        <v>30</v>
-      </c>
-      <c r="J64" t="s">
-        <v>364</v>
-      </c>
-      <c r="K64" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>361</v>
+      </c>
+      <c r="B65" t="s">
+        <v>362</v>
+      </c>
+      <c r="C65" t="s">
+        <v>363</v>
+      </c>
+      <c r="D65" t="s">
+        <v>364</v>
+      </c>
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" t="s">
+        <v>365</v>
+      </c>
+      <c r="G65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" t="s">
         <v>366</v>
       </c>
-      <c r="B65" t="s">
+      <c r="I65" t="s">
         <v>367</v>
       </c>
-      <c r="C65" t="s">
+      <c r="J65"/>
+      <c r="K65" t="s">
         <v>368</v>
       </c>
-      <c r="D65" t="s">
-        <v>369</v>
-      </c>
-      <c r="E65" t="s">
-        <v>71</v>
-      </c>
-      <c r="F65" t="s">
-        <v>370</v>
-      </c>
-      <c r="G65" t="s">
-        <v>17</v>
-      </c>
-      <c r="H65" t="s">
-        <v>73</v>
-      </c>
-      <c r="I65" t="s">
-        <v>30</v>
-      </c>
-      <c r="J65" t="s">
-        <v>371</v>
-      </c>
-      <c r="K65"/>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>369</v>
+      </c>
+      <c r="B66" t="s">
+        <v>370</v>
+      </c>
+      <c r="C66" t="s">
+        <v>371</v>
+      </c>
+      <c r="D66" t="s">
         <v>372</v>
       </c>
-      <c r="B66" t="s">
+      <c r="E66" t="s">
+        <v>89</v>
+      </c>
+      <c r="F66" t="s">
         <v>373</v>
       </c>
-      <c r="C66" t="s">
+      <c r="G66" t="s">
+        <v>302</v>
+      </c>
+      <c r="H66" t="s">
+        <v>219</v>
+      </c>
+      <c r="I66" t="s">
+        <v>30</v>
+      </c>
+      <c r="J66" t="s">
         <v>374</v>
       </c>
-      <c r="D66" t="s">
+      <c r="K66" t="s">
         <v>375</v>
       </c>
-      <c r="E66" t="s">
-        <v>79</v>
-      </c>
-      <c r="F66" t="s">
-        <v>376</v>
-      </c>
-      <c r="G66" t="s">
-        <v>377</v>
-      </c>
-      <c r="H66" t="s">
-        <v>209</v>
-      </c>
-      <c r="I66" t="s">
-        <v>378</v>
-      </c>
-      <c r="J66" t="s">
-        <v>379</v>
-      </c>
-      <c r="K66"/>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>376</v>
+      </c>
+      <c r="B67" t="s">
+        <v>377</v>
+      </c>
+      <c r="C67" t="s">
+        <v>378</v>
+      </c>
+      <c r="D67" t="s">
+        <v>379</v>
+      </c>
+      <c r="E67" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" t="s">
         <v>380</v>
       </c>
-      <c r="B67" t="s">
-        <v>381</v>
-      </c>
-      <c r="C67" t="s">
-        <v>382</v>
-      </c>
-      <c r="D67" t="s">
-        <v>383</v>
-      </c>
-      <c r="E67" t="s">
-        <v>71</v>
-      </c>
-      <c r="F67" t="s">
-        <v>339</v>
-      </c>
       <c r="G67" t="s">
-        <v>277</v>
+        <v>17</v>
       </c>
       <c r="H67" t="s">
-        <v>209</v>
+        <v>80</v>
       </c>
       <c r="I67" t="s">
         <v>30</v>
       </c>
       <c r="J67" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="K67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>382</v>
+      </c>
+      <c r="B68" t="s">
+        <v>383</v>
+      </c>
+      <c r="C68" t="s">
+        <v>384</v>
+      </c>
+      <c r="D68" t="s">
         <v>385</v>
       </c>
-      <c r="B68" t="s">
+      <c r="E68" t="s">
+        <v>89</v>
+      </c>
+      <c r="F68" t="s">
         <v>386</v>
       </c>
-      <c r="C68" t="s">
+      <c r="G68" t="s">
         <v>387</v>
       </c>
-      <c r="D68" t="s">
+      <c r="H68" t="s">
+        <v>219</v>
+      </c>
+      <c r="I68" t="s">
         <v>388</v>
       </c>
-      <c r="E68" t="s">
-        <v>71</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="J68" t="s">
         <v>389</v>
-      </c>
-      <c r="G68" t="s">
-        <v>17</v>
-      </c>
-      <c r="H68" t="s">
-        <v>390</v>
-      </c>
-      <c r="I68" t="s">
-        <v>30</v>
-      </c>
-      <c r="J68" t="s">
-        <v>391</v>
       </c>
       <c r="K68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>390</v>
+      </c>
+      <c r="B69" t="s">
+        <v>391</v>
+      </c>
+      <c r="C69" t="s">
         <v>392</v>
       </c>
-      <c r="B69" t="s">
+      <c r="D69" t="s">
         <v>393</v>
       </c>
-      <c r="C69"/>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" t="s">
+        <v>349</v>
+      </c>
+      <c r="G69" t="s">
+        <v>287</v>
+      </c>
+      <c r="H69" t="s">
+        <v>219</v>
+      </c>
+      <c r="I69" t="s">
+        <v>30</v>
+      </c>
+      <c r="J69" t="s">
         <v>394</v>
       </c>
-      <c r="E69" t="s">
-        <v>71</v>
-      </c>
-      <c r="F69" t="s">
-        <v>393</v>
-      </c>
-      <c r="G69" t="s">
-        <v>395</v>
-      </c>
-      <c r="H69" t="s">
-        <v>81</v>
-      </c>
-      <c r="I69" t="s">
-        <v>396</v>
-      </c>
-      <c r="J69"/>
-      <c r="K69" t="s">
-        <v>397</v>
-      </c>
+      <c r="K69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>395</v>
+      </c>
+      <c r="B70" t="s">
+        <v>396</v>
+      </c>
+      <c r="C70" t="s">
+        <v>397</v>
+      </c>
+      <c r="D70" t="s">
         <v>398</v>
       </c>
-      <c r="B70" t="s">
+      <c r="E70" t="s">
+        <v>49</v>
+      </c>
+      <c r="F70" t="s">
         <v>399</v>
-      </c>
-      <c r="C70" t="s">
-        <v>400</v>
-      </c>
-      <c r="D70" t="s">
-        <v>401</v>
-      </c>
-      <c r="E70" t="s">
-        <v>79</v>
-      </c>
-      <c r="F70" t="s">
-        <v>402</v>
       </c>
       <c r="G70" t="s">
         <v>17</v>
       </c>
       <c r="H70" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I70" t="s">
-        <v>404</v>
-      </c>
-      <c r="J70"/>
-      <c r="K70" t="s">
-        <v>405</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="J70" t="s">
+        <v>401</v>
+      </c>
+      <c r="K70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>402</v>
+      </c>
+      <c r="B71" t="s">
+        <v>403</v>
+      </c>
+      <c r="C71"/>
+      <c r="D71" t="s">
+        <v>404</v>
+      </c>
+      <c r="E71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" t="s">
+        <v>403</v>
+      </c>
+      <c r="G71" t="s">
+        <v>405</v>
+      </c>
+      <c r="H71" t="s">
+        <v>91</v>
+      </c>
+      <c r="I71" t="s">
         <v>406</v>
       </c>
-      <c r="B71" t="s">
+      <c r="J71"/>
+      <c r="K71" t="s">
         <v>407</v>
-      </c>
-      <c r="C71" t="s">
-        <v>408</v>
-      </c>
-      <c r="D71" t="s">
-        <v>409</v>
-      </c>
-      <c r="E71" t="s">
-        <v>193</v>
-      </c>
-      <c r="F71" t="s">
-        <v>410</v>
-      </c>
-      <c r="G71" t="s">
-        <v>411</v>
-      </c>
-      <c r="H71" t="s">
-        <v>412</v>
-      </c>
-      <c r="I71" t="s">
-        <v>413</v>
-      </c>
-      <c r="J71" t="s">
-        <v>414</v>
-      </c>
-      <c r="K71" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B72" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C72" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="D72" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E72" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="F72" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="G72" t="s">
-        <v>420</v>
+        <v>17</v>
       </c>
       <c r="H72" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="I72" t="s">
-        <v>422</v>
-      </c>
-      <c r="J72" t="s">
-        <v>423</v>
-      </c>
-      <c r="K72"/>
+        <v>414</v>
+      </c>
+      <c r="J72"/>
+      <c r="K72" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>416</v>
+      </c>
+      <c r="B73" t="s">
+        <v>417</v>
+      </c>
+      <c r="C73" t="s">
+        <v>418</v>
+      </c>
+      <c r="D73" t="s">
+        <v>419</v>
+      </c>
+      <c r="E73" t="s">
+        <v>203</v>
+      </c>
+      <c r="F73" t="s">
+        <v>420</v>
+      </c>
+      <c r="G73" t="s">
+        <v>421</v>
+      </c>
+      <c r="H73" t="s">
+        <v>422</v>
+      </c>
+      <c r="I73" t="s">
+        <v>423</v>
+      </c>
+      <c r="J73" t="s">
         <v>424</v>
       </c>
-      <c r="B73" t="s">
+      <c r="K73" t="s">
         <v>425</v>
       </c>
-      <c r="C73" t="s">
-        <v>426</v>
-      </c>
-      <c r="D73" t="s">
-        <v>427</v>
-      </c>
-      <c r="E73" t="s">
-        <v>43</v>
-      </c>
-      <c r="F73" t="s">
-        <v>428</v>
-      </c>
-      <c r="G73" t="s">
-        <v>17</v>
-      </c>
-      <c r="H73" t="s">
-        <v>174</v>
-      </c>
-      <c r="I73" t="s">
-        <v>30</v>
-      </c>
-      <c r="J73" t="s">
-        <v>429</v>
-      </c>
-      <c r="K73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
+        <v>426</v>
+      </c>
+      <c r="B74" t="s">
+        <v>427</v>
+      </c>
+      <c r="C74" t="s">
+        <v>428</v>
+      </c>
+      <c r="D74" t="s">
+        <v>429</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" t="s">
+        <v>426</v>
+      </c>
+      <c r="G74" t="s">
         <v>430</v>
       </c>
-      <c r="B74" t="s">
+      <c r="H74" t="s">
         <v>431</v>
       </c>
-      <c r="C74" t="s">
+      <c r="I74" t="s">
         <v>432</v>
       </c>
-      <c r="D74" t="s">
+      <c r="J74" t="s">
         <v>433</v>
       </c>
-      <c r="E74" t="s">
-        <v>79</v>
-      </c>
-      <c r="F74" t="s">
-        <v>434</v>
-      </c>
-      <c r="G74" t="s">
-        <v>435</v>
-      </c>
-      <c r="H74" t="s">
-        <v>228</v>
-      </c>
-      <c r="I74" t="s">
-        <v>436</v>
-      </c>
-      <c r="J74" t="s">
-        <v>437</v>
-      </c>
-      <c r="K74" t="s">
-        <v>438</v>
-      </c>
+      <c r="K74"/>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B75" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C75" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D75" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E75" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G75" t="s">
         <v>17</v>
       </c>
       <c r="H75" t="s">
-        <v>443</v>
+        <v>184</v>
       </c>
       <c r="I75" t="s">
         <v>30</v>
       </c>
       <c r="J75" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="K75"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>440</v>
+      </c>
+      <c r="B76" t="s">
+        <v>441</v>
+      </c>
+      <c r="C76" t="s">
+        <v>442</v>
+      </c>
+      <c r="D76" t="s">
+        <v>443</v>
+      </c>
+      <c r="E76" t="s">
+        <v>89</v>
+      </c>
+      <c r="F76" t="s">
+        <v>444</v>
+      </c>
+      <c r="G76" t="s">
         <v>445</v>
       </c>
-      <c r="B76"/>
-      <c r="C76" t="s">
+      <c r="H76" t="s">
+        <v>238</v>
+      </c>
+      <c r="I76" t="s">
         <v>446</v>
       </c>
-      <c r="D76" t="s">
+      <c r="J76" t="s">
         <v>447</v>
       </c>
-      <c r="E76" t="s">
+      <c r="K76" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>449</v>
+      </c>
+      <c r="B77" t="s">
+        <v>450</v>
+      </c>
+      <c r="C77" t="s">
+        <v>451</v>
+      </c>
+      <c r="D77" t="s">
+        <v>452</v>
+      </c>
+      <c r="E77" t="s">
+        <v>89</v>
+      </c>
+      <c r="F77" t="s">
+        <v>449</v>
+      </c>
+      <c r="G77" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" t="s">
+        <v>453</v>
+      </c>
+      <c r="I77" t="s">
+        <v>30</v>
+      </c>
+      <c r="J77" t="s">
+        <v>454</v>
+      </c>
+      <c r="K77"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>455</v>
+      </c>
+      <c r="B78"/>
+      <c r="C78" t="s">
+        <v>456</v>
+      </c>
+      <c r="D78" t="s">
+        <v>457</v>
+      </c>
+      <c r="E78" t="s">
         <v>26</v>
       </c>
-      <c r="F76" t="s">
-        <v>448</v>
-      </c>
-      <c r="G76" t="s">
-        <v>167</v>
-      </c>
-      <c r="H76" t="s">
-        <v>449</v>
-      </c>
-      <c r="I76" t="s">
-        <v>348</v>
-      </c>
-      <c r="J76" t="s">
-        <v>450</v>
-      </c>
-      <c r="K76"/>
+      <c r="F78" t="s">
+        <v>458</v>
+      </c>
+      <c r="G78" t="s">
+        <v>177</v>
+      </c>
+      <c r="H78" t="s">
+        <v>459</v>
+      </c>
+      <c r="I78" t="s">
+        <v>358</v>
+      </c>
+      <c r="J78" t="s">
+        <v>460</v>
+      </c>
+      <c r="K78"/>
+    </row>
+    <row r="79">
+      <c r="A79"/>
+      <c r="B79" t="s">
+        <v>46</v>
+      </c>
+      <c r="C79" t="s">
+        <v>47</v>
+      </c>
+      <c r="D79" t="s">
+        <v>461</v>
+      </c>
+      <c r="E79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" t="s">
+        <v>50</v>
+      </c>
+      <c r="G79" t="s">
+        <v>17</v>
+      </c>
+      <c r="H79"/>
+      <c r="I79"/>
+      <c r="J79" t="s">
+        <v>52</v>
+      </c>
+      <c r="K79"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4107,482 +3950,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="50.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>451</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" t="s">
-        <v>454</v>
-      </c>
-      <c r="G2" t="s">
-        <v>455</v>
-      </c>
-      <c r="H2" t="s">
-        <v>456</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>457</v>
-      </c>
-      <c r="K2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>458</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3" t="s">
-        <v>459</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" t="s">
-        <v>460</v>
-      </c>
-      <c r="G3" t="s">
-        <v>461</v>
-      </c>
-      <c r="H3" t="s">
-        <v>462</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>463</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4" t="s">
-        <v>464</v>
-      </c>
-      <c r="D4" t="s">
-        <v>465</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>463</v>
-      </c>
-      <c r="G4" t="s">
-        <v>455</v>
-      </c>
-      <c r="H4" t="s">
-        <v>466</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>467</v>
-      </c>
-      <c r="K4"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>468</v>
-      </c>
-      <c r="B5" t="s">
-        <v>469</v>
-      </c>
-      <c r="C5" t="s">
-        <v>470</v>
-      </c>
-      <c r="D5" t="s">
-        <v>471</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>472</v>
-      </c>
-      <c r="G5" t="s">
-        <v>455</v>
-      </c>
-      <c r="H5" t="s">
-        <v>473</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>474</v>
-      </c>
-      <c r="B6"/>
-      <c r="C6" t="s">
-        <v>475</v>
-      </c>
-      <c r="D6" t="s">
-        <v>476</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>477</v>
-      </c>
-      <c r="G6" t="s">
-        <v>455</v>
-      </c>
-      <c r="H6" t="s">
-        <v>456</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" t="s">
-        <v>478</v>
-      </c>
-      <c r="K6"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>479</v>
-      </c>
-      <c r="B7" t="s">
-        <v>480</v>
-      </c>
-      <c r="C7" t="s">
-        <v>481</v>
-      </c>
-      <c r="D7" t="s">
-        <v>482</v>
-      </c>
-      <c r="E7" t="s">
-        <v>483</v>
-      </c>
-      <c r="F7" t="s">
-        <v>484</v>
-      </c>
-      <c r="G7" t="s">
-        <v>485</v>
-      </c>
-      <c r="H7" t="s">
-        <v>486</v>
-      </c>
-      <c r="I7" t="s">
-        <v>487</v>
-      </c>
-      <c r="J7" t="s">
-        <v>488</v>
-      </c>
-      <c r="K7" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>490</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8" t="s">
-        <v>491</v>
-      </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" t="s">
-        <v>490</v>
-      </c>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>492</v>
-      </c>
-      <c r="B9" t="s">
-        <v>493</v>
-      </c>
-      <c r="C9" t="s">
-        <v>494</v>
-      </c>
-      <c r="D9" t="s">
-        <v>495</v>
-      </c>
-      <c r="E9" t="s">
-        <v>496</v>
-      </c>
-      <c r="F9" t="s">
-        <v>497</v>
-      </c>
-      <c r="G9" t="s">
-        <v>498</v>
-      </c>
-      <c r="H9" t="s">
-        <v>499</v>
-      </c>
-      <c r="I9" t="s">
-        <v>500</v>
-      </c>
-      <c r="J9" t="s">
-        <v>501</v>
-      </c>
-      <c r="K9" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>503</v>
-      </c>
-      <c r="B10"/>
-      <c r="C10" t="s">
-        <v>504</v>
-      </c>
-      <c r="D10" t="s">
-        <v>505</v>
-      </c>
-      <c r="E10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" t="s">
-        <v>506</v>
-      </c>
-      <c r="G10" t="s">
-        <v>455</v>
-      </c>
-      <c r="H10" t="s">
-        <v>456</v>
-      </c>
-      <c r="I10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" t="s">
-        <v>507</v>
-      </c>
-      <c r="K10"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>508</v>
-      </c>
-      <c r="B11" t="s">
-        <v>509</v>
-      </c>
-      <c r="C11" t="s">
-        <v>510</v>
-      </c>
-      <c r="D11" t="s">
-        <v>511</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>512</v>
-      </c>
-      <c r="G11" t="s">
-        <v>461</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11" t="s">
-        <v>513</v>
-      </c>
-      <c r="K11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="50.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>514</v>
-      </c>
-      <c r="B2" t="s">
-        <v>515</v>
-      </c>
-      <c r="C2" t="s">
-        <v>516</v>
-      </c>
-      <c r="D2" t="s">
-        <v>517</v>
-      </c>
-      <c r="E2" t="s">
-        <v>518</v>
-      </c>
-      <c r="F2" t="s">
-        <v>519</v>
-      </c>
-      <c r="G2" t="s">
-        <v>498</v>
-      </c>
-      <c r="H2" t="s">
-        <v>520</v>
-      </c>
-      <c r="I2" t="s">
-        <v>521</v>
-      </c>
-      <c r="J2" t="s">
-        <v>522</v>
-      </c>
-      <c r="K2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>524</v>
-      </c>
-      <c r="B3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C3" t="s">
-        <v>526</v>
-      </c>
-      <c r="D3" t="s">
-        <v>527</v>
-      </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G3" t="s">
-        <v>498</v>
-      </c>
-      <c r="H3" t="s">
-        <v>528</v>
-      </c>
-      <c r="I3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3" t="s">
-        <v>529</v>
-      </c>
-      <c r="K3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId5"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>